<commit_message>
add similarity in excel tools
</commit_message>
<xml_diff>
--- a/7930_tools.xlsx
+++ b/7930_tools.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/xxb/Desktop/Practice/001_hkbu_2_final_exam/7930_BDA_exam/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FC4B5F5A-50FE-874B-BF67-E66BEB09C5BD}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D37BE426-78C7-8D42-B144-F488E5C7F983}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1800" yWindow="1840" windowWidth="29600" windowHeight="19200" xr2:uid="{55DB38B1-E4A7-46EC-8B7A-8D5782EED99B}"/>
+    <workbookView xWindow="1800" yWindow="580" windowWidth="29600" windowHeight="19200" xr2:uid="{55DB38B1-E4A7-46EC-8B7A-8D5782EED99B}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="28">
   <si>
     <t>X</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -83,6 +83,60 @@
     <t>L = 1</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
+  <si>
+    <t>similarity</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>A</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>B</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>C</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>D</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>E</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>H1</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>H2</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>H3</t>
+  </si>
+  <si>
+    <t>H4</t>
+  </si>
+  <si>
+    <t>H5</t>
+  </si>
+  <si>
+    <t>H6</t>
+  </si>
+  <si>
+    <t>H7</t>
+  </si>
+  <si>
+    <t>H8</t>
+  </si>
+  <si>
+    <t>mean</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
 </sst>
 </file>
 
@@ -114,7 +168,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="6">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -145,13 +199,37 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="3">
     <border>
       <left/>
       <right/>
       <top/>
       <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
       <diagonal/>
     </border>
   </borders>
@@ -160,7 +238,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -177,6 +255,21 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="2" xfId="0" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -2036,14 +2129,14 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>9</xdr:col>
-      <xdr:colOff>144379</xdr:colOff>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>165028</xdr:colOff>
       <xdr:row>0</xdr:row>
       <xdr:rowOff>112962</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>16</xdr:col>
-      <xdr:colOff>57484</xdr:colOff>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>78133</xdr:colOff>
       <xdr:row>22</xdr:row>
       <xdr:rowOff>117642</xdr:rowOff>
     </xdr:to>
@@ -2072,16 +2165,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>9</xdr:col>
-      <xdr:colOff>36094</xdr:colOff>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>159994</xdr:colOff>
       <xdr:row>23</xdr:row>
       <xdr:rowOff>74863</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>15</xdr:col>
-      <xdr:colOff>284479</xdr:colOff>
-      <xdr:row>45</xdr:row>
-      <xdr:rowOff>101600</xdr:rowOff>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>408378</xdr:colOff>
+      <xdr:row>42</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -2406,10 +2499,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5E17D757-4C73-4CA4-9ECF-DF2B53F429AE}">
-  <dimension ref="A1:I31"/>
+  <dimension ref="A1:J40"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="125" zoomScaleNormal="190" workbookViewId="0">
-      <selection activeCell="G11" sqref="G11"/>
+    <sheetView tabSelected="1" topLeftCell="A16" zoomScale="123" zoomScaleNormal="190" workbookViewId="0">
+      <selection activeCell="H44" sqref="H44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
@@ -2460,11 +2553,11 @@
         <v>10</v>
       </c>
       <c r="E3" s="1">
-        <f>(B3-$B$16)^2+(C3-$C$16)^2</f>
+        <f t="shared" ref="E3:E9" si="0">(B3-$B$16)^2+(C3-$C$16)^2</f>
         <v>0</v>
       </c>
       <c r="F3" s="1">
-        <f>(B3-$B$17)^2+(C3-$C$17)^2</f>
+        <f t="shared" ref="F3:F9" si="1">(B3-$B$17)^2+(C3-$C$17)^2</f>
         <v>73</v>
       </c>
       <c r="H3" s="1">
@@ -2487,19 +2580,19 @@
         <v>5</v>
       </c>
       <c r="E4" s="1">
-        <f>(B4-$B$16)^2+(C4-$C$16)^2</f>
+        <f t="shared" si="0"/>
         <v>25</v>
       </c>
       <c r="F4" s="1">
-        <f>(B4-$B$17)^2+(C4-$C$17)^2</f>
+        <f t="shared" si="1"/>
         <v>18</v>
       </c>
       <c r="H4" s="1">
-        <f t="shared" ref="H4:H10" si="0">ABS(B4-$B$16)+ABS(C4-$C$16)</f>
+        <f t="shared" ref="H4:H10" si="2">ABS(B4-$B$16)+ABS(C4-$C$16)</f>
         <v>5</v>
       </c>
       <c r="I4" s="1">
-        <f t="shared" ref="I4:I10" si="1">ABS(B4-$B$17)+ABS(C4-$C$17)</f>
+        <f t="shared" ref="I4:I10" si="3">ABS(B4-$B$17)+ABS(C4-$C$17)</f>
         <v>6</v>
       </c>
     </row>
@@ -2514,11 +2607,11 @@
         <v>4</v>
       </c>
       <c r="E5" s="1">
-        <f>(B5-$B$16)^2+(C5-$C$16)^2</f>
+        <f t="shared" si="0"/>
         <v>45</v>
       </c>
       <c r="F5" s="1">
-        <f>(B5-$B$17)^2+(C5-$C$17)^2</f>
+        <f t="shared" si="1"/>
         <v>40</v>
       </c>
       <c r="H5" s="1">
@@ -2541,19 +2634,19 @@
         <v>8</v>
       </c>
       <c r="E6" s="1">
-        <f>(B6-$B$16)^2+(C6-$C$16)^2</f>
+        <f t="shared" si="0"/>
         <v>4</v>
       </c>
       <c r="F6" s="1">
-        <f>(B6-$B$17)^2+(C6-$C$17)^2</f>
+        <f t="shared" si="1"/>
         <v>45</v>
       </c>
       <c r="H6" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>2</v>
       </c>
       <c r="I6" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>9</v>
       </c>
     </row>
@@ -2568,19 +2661,19 @@
         <v>5</v>
       </c>
       <c r="E7" s="1">
-        <f>(B7-$B$16)^2+(C7-$C$16)^2</f>
+        <f t="shared" si="0"/>
         <v>41</v>
       </c>
       <c r="F7" s="1">
-        <f>(B7-$B$17)^2+(C7-$C$17)^2</f>
+        <f t="shared" si="1"/>
         <v>10</v>
       </c>
       <c r="H7" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>9</v>
       </c>
       <c r="I7" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>4</v>
       </c>
     </row>
@@ -2595,19 +2688,19 @@
         <v>4</v>
       </c>
       <c r="E8" s="1">
-        <f>(B8-$B$16)^2+(C8-$C$16)^2</f>
+        <f t="shared" si="0"/>
         <v>52</v>
       </c>
       <c r="F8" s="1">
-        <f>(B8-$B$17)^2+(C8-$C$17)^2</f>
+        <f t="shared" si="1"/>
         <v>5</v>
       </c>
       <c r="H8" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>10</v>
       </c>
       <c r="I8" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>3</v>
       </c>
     </row>
@@ -2622,19 +2715,19 @@
         <v>2</v>
       </c>
       <c r="E9" s="1">
-        <f>(B9-$B$16)^2+(C9-$C$16)^2</f>
+        <f t="shared" si="0"/>
         <v>80</v>
       </c>
       <c r="F9" s="1">
-        <f>(B9-$B$17)^2+(C9-$C$17)^2</f>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="H9" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>12</v>
       </c>
       <c r="I9" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
     </row>
@@ -2644,11 +2737,11 @@
       <c r="E10" s="1"/>
       <c r="F10" s="1"/>
       <c r="H10" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>15</v>
       </c>
       <c r="I10" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>4</v>
       </c>
     </row>
@@ -2700,11 +2793,11 @@
         <v>10</v>
       </c>
       <c r="E23">
-        <f>(B23-$B$31)^2</f>
+        <f t="shared" ref="E23:E29" si="4">(B23-$B$31)^2</f>
         <v>1.6530612244897955</v>
       </c>
       <c r="F23">
-        <f>(C23-$C$31)^2</f>
+        <f t="shared" ref="F23:F29" si="5">(C23-$C$31)^2</f>
         <v>20.897959183673468</v>
       </c>
       <c r="H23">
@@ -2720,15 +2813,15 @@
         <v>5</v>
       </c>
       <c r="E24">
-        <f>(B24-$B$31)^2</f>
+        <f t="shared" si="4"/>
         <v>1.6530612244897955</v>
       </c>
       <c r="F24">
-        <f>(C24-$C$31)^2</f>
+        <f t="shared" si="5"/>
         <v>0.18367346938775531</v>
       </c>
       <c r="H24">
-        <f t="shared" ref="H24:H29" si="2">E24+F24</f>
+        <f t="shared" ref="H24:H29" si="6">E24+F24</f>
         <v>1.8367346938775508</v>
       </c>
     </row>
@@ -2740,15 +2833,15 @@
         <v>8</v>
       </c>
       <c r="E25">
-        <f>(B25-$B$31)^2</f>
+        <f t="shared" si="4"/>
         <v>1.6530612244897955</v>
       </c>
       <c r="F25">
-        <f>(C25-$C$31)^2</f>
+        <f t="shared" si="5"/>
         <v>6.6122448979591821</v>
       </c>
       <c r="H25">
-        <f t="shared" si="2"/>
+        <f t="shared" si="6"/>
         <v>8.2653061224489779</v>
       </c>
     </row>
@@ -2760,15 +2853,15 @@
         <v>5</v>
       </c>
       <c r="E26">
-        <f>(B26-$B$31)^2</f>
+        <f t="shared" si="4"/>
         <v>7.3673469387755111</v>
       </c>
       <c r="F26">
-        <f>(C26-$C$31)^2</f>
+        <f t="shared" si="5"/>
         <v>0.18367346938775531</v>
       </c>
       <c r="H26">
-        <f t="shared" si="2"/>
+        <f t="shared" si="6"/>
         <v>7.5510204081632661</v>
       </c>
     </row>
@@ -2780,15 +2873,15 @@
         <v>4</v>
       </c>
       <c r="E27">
-        <f>(B27-$B$31)^2</f>
+        <f t="shared" si="4"/>
         <v>7.3673469387755111</v>
       </c>
       <c r="F27">
-        <f>(C27-$C$31)^2</f>
+        <f t="shared" si="5"/>
         <v>2.0408163265306132</v>
       </c>
       <c r="H27">
-        <f t="shared" si="2"/>
+        <f t="shared" si="6"/>
         <v>9.4081632653061238</v>
       </c>
     </row>
@@ -2800,15 +2893,15 @@
         <v>2</v>
       </c>
       <c r="E28">
-        <f>(B28-$B$31)^2</f>
+        <f t="shared" si="4"/>
         <v>7.3673469387755111</v>
       </c>
       <c r="F28">
-        <f>(C28-$C$31)^2</f>
+        <f t="shared" si="5"/>
         <v>11.755102040816329</v>
       </c>
       <c r="H28">
-        <f t="shared" si="2"/>
+        <f t="shared" si="6"/>
         <v>19.122448979591841</v>
       </c>
     </row>
@@ -2820,15 +2913,15 @@
         <v>4</v>
       </c>
       <c r="E29">
-        <f>(B29-$B$31)^2</f>
+        <f t="shared" si="4"/>
         <v>18.367346938775508</v>
       </c>
       <c r="F29">
-        <f>(C29-$C$31)^2</f>
+        <f t="shared" si="5"/>
         <v>2.0408163265306132</v>
       </c>
       <c r="H29">
-        <f t="shared" si="2"/>
+        <f t="shared" si="6"/>
         <v>20.408163265306122</v>
       </c>
     </row>
@@ -2851,6 +2944,143 @@
         <f>SUM(H23:H29)</f>
         <v>89.142857142857139</v>
       </c>
+    </row>
+    <row r="34" spans="1:10">
+      <c r="B34" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="35" spans="1:10">
+      <c r="B35" t="s">
+        <v>19</v>
+      </c>
+      <c r="C35" t="s">
+        <v>20</v>
+      </c>
+      <c r="D35" t="s">
+        <v>21</v>
+      </c>
+      <c r="E35" t="s">
+        <v>22</v>
+      </c>
+      <c r="F35" t="s">
+        <v>23</v>
+      </c>
+      <c r="G35" t="s">
+        <v>24</v>
+      </c>
+      <c r="H35" t="s">
+        <v>25</v>
+      </c>
+      <c r="I35" t="s">
+        <v>26</v>
+      </c>
+      <c r="J35" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="36" spans="1:10">
+      <c r="A36" t="s">
+        <v>14</v>
+      </c>
+      <c r="B36" s="7">
+        <v>4</v>
+      </c>
+      <c r="C36" s="7"/>
+      <c r="D36" s="7"/>
+      <c r="E36" s="7">
+        <v>5</v>
+      </c>
+      <c r="F36" s="7">
+        <v>1</v>
+      </c>
+      <c r="G36" s="7"/>
+      <c r="H36" s="7"/>
+      <c r="I36" s="7"/>
+      <c r="J36">
+        <f>AVERAGE(B36:I36)</f>
+        <v>3.3333333333333335</v>
+      </c>
+    </row>
+    <row r="37" spans="1:10" s="9" customFormat="1">
+      <c r="A37" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="B37" s="10">
+        <v>5</v>
+      </c>
+      <c r="C37" s="10">
+        <v>5</v>
+      </c>
+      <c r="D37" s="10">
+        <v>4</v>
+      </c>
+      <c r="E37" s="10"/>
+      <c r="F37" s="10"/>
+      <c r="G37" s="10"/>
+      <c r="H37" s="10"/>
+      <c r="I37" s="10"/>
+      <c r="J37">
+        <f t="shared" ref="J37:J39" si="7">AVERAGE(B37:I37)</f>
+        <v>4.666666666666667</v>
+      </c>
+    </row>
+    <row r="38" spans="1:10">
+      <c r="A38" t="s">
+        <v>16</v>
+      </c>
+      <c r="B38" s="6"/>
+      <c r="C38" s="6"/>
+      <c r="D38" s="6"/>
+      <c r="E38" s="6">
+        <v>2</v>
+      </c>
+      <c r="F38" s="6">
+        <v>4</v>
+      </c>
+      <c r="G38" s="6">
+        <v>5</v>
+      </c>
+      <c r="H38" s="6"/>
+      <c r="I38" s="6"/>
+      <c r="J38">
+        <f t="shared" si="7"/>
+        <v>3.6666666666666665</v>
+      </c>
+    </row>
+    <row r="39" spans="1:10" s="9" customFormat="1">
+      <c r="A39" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="B39" s="10"/>
+      <c r="C39" s="10">
+        <v>3</v>
+      </c>
+      <c r="D39" s="10"/>
+      <c r="E39" s="10"/>
+      <c r="F39" s="10"/>
+      <c r="G39" s="10"/>
+      <c r="H39" s="10">
+        <v>3</v>
+      </c>
+      <c r="I39" s="10"/>
+      <c r="J39">
+        <f t="shared" si="7"/>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="40" spans="1:10">
+      <c r="A40" t="s">
+        <v>18</v>
+      </c>
+      <c r="B40" s="8"/>
+      <c r="C40" s="8"/>
+      <c r="D40" s="8"/>
+      <c r="E40" s="8"/>
+      <c r="F40" s="8"/>
+      <c r="G40" s="8"/>
+      <c r="H40" s="8"/>
+      <c r="I40" s="8"/>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>

</xml_diff>